<commit_message>
Code review comment completed : Add SonarLint plugin & fix all blocker & major issues.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/cleartrip_testdata.xlsx
+++ b/src/test/resources/data/cleartrip_testdata.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0CB1735C-D594-4707-BB79-22A171750BE3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B386E439-C48C-4575-8AEF-7DD86D6BA2E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="5160" xr2:uid="{4573F608-46D1-48CC-95B8-5B6B0B834336}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18030" windowHeight="6705" activeTab="2" xr2:uid="{4573F608-46D1-48CC-95B8-5B6B0B834336}"/>
   </bookViews>
   <sheets>
     <sheet name="searchFlight_OneWay" sheetId="1" r:id="rId1"/>
     <sheet name="searchFlight_RoundTrip" sheetId="2" r:id="rId2"/>
+    <sheet name="restServiceForCleartrip" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N15"/>
+  <oleSize ref="A1:R20"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>source</t>
   </si>
@@ -52,6 +53,57 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>trip_type</t>
+  </si>
+  <si>
+    <t>depart_date</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>ver</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>ONEWAY</t>
+  </si>
+  <si>
+    <t>Mumbai IN Chatrapati Shivaji Airport (BOM)</t>
+  </si>
+  <si>
+    <t>25/10/2018</t>
+  </si>
+  <si>
+    <t>Pune%2C+IN+-+Lohegaon+(PNQ)</t>
+  </si>
+  <si>
+    <t>PNQ</t>
+  </si>
+  <si>
+    <t>BOM</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>class1</t>
   </si>
 </sst>
 </file>
@@ -405,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BE054B-2FC9-4760-A658-C1C44C9A54A9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -532,4 +584,108 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B9D6C31-29FA-4F49-9E29-E7DCBC6B69E0}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>